<commit_message>
- Dump based database - Fixed hours to fit schedule - First draft of backend for game
</commit_message>
<xml_diff>
--- a/doc/Horaire.xlsx
+++ b/doc/Horaire.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fred\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\actimania\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18110"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18113"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="53">
   <si>
     <t>Bleus</t>
   </si>
@@ -108,15 +108,94 @@
   </si>
   <si>
     <t>Vendredi</t>
+  </si>
+  <si>
+    <t>Marymount Academy</t>
+  </si>
+  <si>
+    <t>John Abbott College</t>
+  </si>
+  <si>
+    <t>Collège de Bois-de-Boulogne</t>
+  </si>
+  <si>
+    <t>Collège Montmorency</t>
+  </si>
+  <si>
+    <t>E.C.S</t>
+  </si>
+  <si>
+    <t>West Island College</t>
+  </si>
+  <si>
+    <t>Marianopolis College</t>
+  </si>
+  <si>
+    <t>Macdonald High School</t>
+  </si>
+  <si>
+    <t>école secondaire Curé-Antoine-Labelle</t>
+  </si>
+  <si>
+    <t>Collège Notre-Dame 1</t>
+  </si>
+  <si>
+    <t>College citoyen</t>
+  </si>
+  <si>
+    <t>Dawson College</t>
+  </si>
+  <si>
+    <t>Collège Laval</t>
+  </si>
+  <si>
+    <t>St. George's School of Montreal</t>
+  </si>
+  <si>
+    <t>Collège Notre-Dame 2</t>
+  </si>
+  <si>
+    <t>Centennial Academy</t>
+  </si>
+  <si>
+    <t>Collège Sainte-Marcelline</t>
+  </si>
+  <si>
+    <t>Cégep Gérald Godin</t>
+  </si>
+  <si>
+    <t>Laval Senior Academy</t>
+  </si>
+  <si>
+    <t>Bialik High School</t>
+  </si>
+  <si>
+    <t>Cégep Vanier College</t>
+  </si>
+  <si>
+    <t>Lake of Two Mountains High School</t>
+  </si>
+  <si>
+    <t>Selwyn House School</t>
+  </si>
+  <si>
+    <t>Bishop's College School</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -131,7 +210,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -355,11 +434,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -409,6 +501,9 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -422,6 +517,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -731,42 +836,42 @@
   <dimension ref="A2:AZ57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="3" width="11.453125" style="1"/>
-    <col min="4" max="7" width="27.7265625" style="1" customWidth="1"/>
-    <col min="8" max="51" width="11.453125" customWidth="1"/>
-    <col min="52" max="52" width="10.90625" customWidth="1"/>
-    <col min="53" max="16384" width="11.453125" style="1"/>
+    <col min="1" max="3" width="11.46484375" style="1"/>
+    <col min="4" max="7" width="27.73046875" style="1" customWidth="1"/>
+    <col min="8" max="51" width="11.46484375" customWidth="1"/>
+    <col min="52" max="52" width="10.9296875" customWidth="1"/>
+    <col min="53" max="16384" width="11.46484375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+    </row>
+    <row r="3" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="2"/>
       <c r="C3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19" t="s">
+      <c r="E3" s="26"/>
+      <c r="F3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="18"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
+      <c r="G3" s="26"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A4" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="16">
@@ -775,260 +880,260 @@
       <c r="C4" s="10">
         <v>1</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="20"/>
+      <c r="D4" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A5" s="21"/>
       <c r="B5" s="16">
         <v>0.77777777777777779</v>
       </c>
       <c r="C5" s="11">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="20"/>
+      <c r="D5" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A6" s="21"/>
       <c r="B6" s="16">
         <v>0.78472222222222199</v>
       </c>
       <c r="C6" s="11">
         <v>3</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="20"/>
+      <c r="D6" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A7" s="21"/>
       <c r="B7" s="16">
         <v>0.79166666666666696</v>
       </c>
       <c r="C7" s="11">
         <v>4</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="20"/>
+      <c r="D7" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A8" s="21"/>
       <c r="B8" s="16">
         <v>0.79861111111111105</v>
       </c>
       <c r="C8" s="11">
         <v>5</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="20"/>
+      <c r="D8" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A9" s="21"/>
       <c r="B9" s="16">
         <v>0.80555555555555503</v>
       </c>
       <c r="C9" s="11">
         <v>6</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="20"/>
+      <c r="D9" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A10" s="21"/>
       <c r="B10" s="16">
         <v>0.8125</v>
       </c>
       <c r="C10" s="11">
         <v>7</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="20"/>
+      <c r="D10" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A11" s="21"/>
       <c r="B11" s="16">
         <v>0.81944444444444398</v>
       </c>
       <c r="C11" s="11">
         <v>8</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="20"/>
+      <c r="D11" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A12" s="21"/>
       <c r="B12" s="16">
         <v>0.82638888888888895</v>
       </c>
       <c r="C12" s="11">
         <v>9</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="20"/>
+      <c r="D12" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A13" s="21"/>
       <c r="B13" s="16">
         <v>0.83333333333333304</v>
       </c>
       <c r="C13" s="11">
         <v>10</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="20"/>
+      <c r="D13" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A14" s="21"/>
       <c r="B14" s="16">
         <v>0.84027777777777801</v>
       </c>
       <c r="C14" s="11">
         <v>11</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="20"/>
+      <c r="D14" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A15" s="21"/>
       <c r="B15" s="16">
         <v>0.84722222222222199</v>
       </c>
       <c r="C15" s="11">
         <v>12</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D15" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="21" t="s">
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A17" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="16">
@@ -1037,795 +1142,795 @@
       <c r="C17" s="11">
         <v>13</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="21"/>
+      <c r="D17" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A18" s="22"/>
       <c r="B18" s="16">
         <v>0.38194444444444442</v>
       </c>
       <c r="C18" s="11">
         <v>14</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="21"/>
+      <c r="D18" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A19" s="22"/>
       <c r="B19" s="16">
         <v>0.38888888888888901</v>
       </c>
       <c r="C19" s="11">
         <v>15</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="21"/>
+      <c r="D19" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A20" s="22"/>
       <c r="B20" s="16">
         <v>0.39583333333333298</v>
       </c>
       <c r="C20" s="11">
         <v>16</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="21"/>
+      <c r="D20" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A21" s="22"/>
       <c r="B21" s="16">
         <v>0.40277777777777801</v>
       </c>
       <c r="C21" s="11">
         <v>17</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="21"/>
+      <c r="D21" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A22" s="22"/>
       <c r="B22" s="16">
         <v>0.40972222222222199</v>
       </c>
       <c r="C22" s="11">
         <v>18</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="21"/>
+      <c r="D22" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A23" s="22"/>
       <c r="B23" s="16">
         <v>0.41666666666666702</v>
       </c>
       <c r="C23" s="11">
         <v>19</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="21"/>
+      <c r="D23" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A24" s="22"/>
       <c r="B24" s="16">
         <v>0.42361111111111099</v>
       </c>
       <c r="C24" s="11">
         <v>20</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="21"/>
+      <c r="D24" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A25" s="22"/>
       <c r="B25" s="16">
         <v>0.43055555555555503</v>
       </c>
       <c r="C25" s="11">
         <v>21</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="21"/>
+      <c r="D25" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A26" s="22"/>
       <c r="B26" s="16">
         <v>0.4375</v>
       </c>
       <c r="C26" s="11">
         <v>22</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="21"/>
+      <c r="D26" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A27" s="22"/>
       <c r="B27" s="16">
         <v>0.44444444444444398</v>
       </c>
       <c r="C27" s="11">
         <v>23</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="21"/>
+      <c r="D27" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A28" s="22"/>
       <c r="B28" s="16">
         <v>0.45138888888888901</v>
       </c>
       <c r="C28" s="11">
         <v>24</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="21"/>
+      <c r="D28" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A29" s="22"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="21"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A30" s="22"/>
       <c r="B30" s="16">
         <v>0.54166666666666663</v>
       </c>
       <c r="C30" s="11">
         <v>25</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="21"/>
+      <c r="D30" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A31" s="22"/>
       <c r="B31" s="16">
         <v>0.54861111111111105</v>
       </c>
       <c r="C31" s="11">
         <v>26</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="21"/>
+      <c r="D31" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A32" s="22"/>
       <c r="B32" s="16">
         <v>0.55555555555555503</v>
       </c>
       <c r="C32" s="11">
         <v>27</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="21"/>
+      <c r="D32" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A33" s="22"/>
       <c r="B33" s="16">
         <v>0.5625</v>
       </c>
       <c r="C33" s="11">
         <v>28</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="21"/>
+      <c r="D33" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A34" s="22"/>
       <c r="B34" s="16">
         <v>0.56944444444444398</v>
       </c>
       <c r="C34" s="11">
         <v>29</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="21"/>
+      <c r="D34" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="G34" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A35" s="22"/>
       <c r="B35" s="16">
         <v>0.57638888888888895</v>
       </c>
       <c r="C35" s="11">
         <v>30</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="21"/>
+      <c r="D35" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G35" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A36" s="22"/>
       <c r="B36" s="16">
         <v>0.58333333333333304</v>
       </c>
       <c r="C36" s="11">
         <v>31</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="21"/>
+      <c r="D36" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G36" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A37" s="22"/>
       <c r="B37" s="16">
         <v>0.59027777777777801</v>
       </c>
       <c r="C37" s="11">
         <v>32</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="21"/>
+      <c r="D37" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G37" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A38" s="22"/>
       <c r="B38" s="16">
         <v>0.59722222222222199</v>
       </c>
       <c r="C38" s="11">
         <v>33</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="21"/>
+      <c r="D38" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A39" s="22"/>
       <c r="B39" s="16">
         <v>0.60416666666666596</v>
       </c>
       <c r="C39" s="11">
         <v>34</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="21"/>
+      <c r="D39" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G39" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A40" s="22"/>
       <c r="B40" s="16">
         <v>0.61111111111111105</v>
       </c>
       <c r="C40" s="11">
         <v>35</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="21"/>
+      <c r="D40" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G40" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A41" s="22"/>
       <c r="B41" s="16">
         <v>0.61805555555555503</v>
       </c>
       <c r="C41" s="11">
         <v>36</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F41" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="21"/>
+      <c r="D41" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E41" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G41" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A42" s="22"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="21"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A43" s="22"/>
       <c r="B43" s="16">
         <v>0.75</v>
       </c>
       <c r="C43" s="11">
         <v>37</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="21"/>
+      <c r="D43" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G43" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A44" s="22"/>
       <c r="B44" s="16">
         <v>0.75694444444444453</v>
       </c>
       <c r="C44" s="11">
         <v>38</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="21"/>
+      <c r="D44" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G44" s="23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A45" s="22"/>
       <c r="B45" s="16">
         <v>0.76388888888888895</v>
       </c>
       <c r="C45" s="11">
         <v>39</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="21"/>
+      <c r="D45" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F45" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G45" s="23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A46" s="22"/>
       <c r="B46" s="16">
         <v>0.77083333333333404</v>
       </c>
       <c r="C46" s="11">
         <v>40</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F46" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="21"/>
+      <c r="D46" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F46" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G46" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A47" s="22"/>
       <c r="B47" s="16">
         <v>0.77777777777777801</v>
       </c>
       <c r="C47" s="11">
         <v>41</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F47" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="21"/>
+      <c r="D47" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G47" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A48" s="22"/>
       <c r="B48" s="16">
         <v>0.78472222222222299</v>
       </c>
       <c r="C48" s="11">
         <v>42</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F48" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="21"/>
+      <c r="D48" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G48" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A49" s="22"/>
       <c r="B49" s="16">
         <v>0.79166666666666696</v>
       </c>
       <c r="C49" s="11">
         <v>43</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" s="21"/>
+      <c r="D49" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E49" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F49" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G49" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A50" s="22"/>
       <c r="B50" s="16">
         <v>0.79861111111111205</v>
       </c>
       <c r="C50" s="11">
         <v>44</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" s="21"/>
+      <c r="D50" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F50" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G50" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A51" s="22"/>
       <c r="B51" s="16">
         <v>0.80555555555555602</v>
       </c>
       <c r="C51" s="11">
         <v>45</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F51" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="21"/>
+      <c r="D51" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F51" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G51" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A52" s="22"/>
       <c r="B52" s="16">
         <v>0.812500000000001</v>
       </c>
       <c r="C52" s="11">
         <v>46</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="21"/>
+      <c r="D52" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F52" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G52" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A53" s="22"/>
       <c r="B53" s="16">
         <v>0.81944444444444497</v>
       </c>
       <c r="C53" s="11">
         <v>47</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F53" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="21"/>
+      <c r="D53" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E53" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F53" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G53" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="22"/>
       <c r="B54" s="16">
         <v>0.82638888888888995</v>
       </c>
       <c r="C54" s="12">
         <v>48</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D54" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F54" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G54" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1847,31 +1952,31 @@
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="11.453125" style="2"/>
-    <col min="3" max="6" width="27.7265625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" customWidth="1"/>
-    <col min="10" max="16384" width="11.453125" style="2"/>
+    <col min="1" max="2" width="11.46484375" style="2"/>
+    <col min="3" max="6" width="27.73046875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.46484375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.46484375" customWidth="1"/>
+    <col min="9" max="9" width="10.9296875" customWidth="1"/>
+    <col min="10" max="16384" width="11.46484375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="18"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="16">
         <v>0.77083333333333337</v>
       </c>
@@ -1891,7 +1996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="16">
         <v>0.77777777777777779</v>
       </c>
@@ -1911,7 +2016,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="16">
         <v>0.78472222222222199</v>
       </c>
@@ -1931,7 +2036,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="16">
         <v>0.79166666666666696</v>
       </c>
@@ -1951,7 +2056,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="16">
         <v>0.79861111111111105</v>
       </c>
@@ -1971,7 +2076,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="16">
         <v>0.80555555555555503</v>
       </c>
@@ -1991,7 +2096,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="16">
         <v>0.8125</v>
       </c>
@@ -2011,7 +2116,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="16">
         <v>0.81944444444444398</v>
       </c>
@@ -2031,7 +2136,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="16">
         <v>0.82638888888888895</v>
       </c>
@@ -2051,7 +2156,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="16">
         <v>0.83333333333333304</v>
       </c>
@@ -2071,7 +2176,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="16">
         <v>0.84027777777777801</v>
       </c>
@@ -2091,7 +2196,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="16">
         <v>0.84722222222222199</v>
       </c>
@@ -2111,7 +2216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="16">
         <v>0.375</v>
       </c>
@@ -2131,7 +2236,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="16">
         <v>0.38194444444444442</v>
       </c>
@@ -2151,7 +2256,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="16">
         <v>0.38888888888888901</v>
       </c>
@@ -2171,7 +2276,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="16">
         <v>0.39583333333333298</v>
       </c>
@@ -2191,7 +2296,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="16">
         <v>0.40277777777777801</v>
       </c>
@@ -2211,7 +2316,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="16">
         <v>0.40972222222222199</v>
       </c>
@@ -2231,7 +2336,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="16">
         <v>0.41666666666666702</v>
       </c>
@@ -2251,7 +2356,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="16">
         <v>0.42361111111111099</v>
       </c>
@@ -2271,7 +2376,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="16">
         <v>0.43055555555555503</v>
       </c>
@@ -2291,7 +2396,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="16">
         <v>0.4375</v>
       </c>
@@ -2311,7 +2416,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="16">
         <v>0.44444444444444398</v>
       </c>
@@ -2331,7 +2436,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="16">
         <v>0.45138888888888901</v>
       </c>
@@ -2351,7 +2456,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="16">
         <v>0.54166666666666663</v>
       </c>
@@ -2371,7 +2476,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="16">
         <v>0.54861111111111105</v>
       </c>
@@ -2391,7 +2496,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="16">
         <v>0.55555555555555503</v>
       </c>
@@ -2411,7 +2516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="16">
         <v>0.5625</v>
       </c>
@@ -2431,7 +2536,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="16">
         <v>0.56944444444444398</v>
       </c>
@@ -2451,7 +2556,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="16">
         <v>0.57638888888888895</v>
       </c>
@@ -2471,7 +2576,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="16">
         <v>0.58333333333333304</v>
       </c>
@@ -2491,7 +2596,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="16">
         <v>0.59027777777777801</v>
       </c>
@@ -2511,7 +2616,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="16">
         <v>0.59722222222222199</v>
       </c>
@@ -2531,7 +2636,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="16">
         <v>0.60416666666666596</v>
       </c>
@@ -2551,7 +2656,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="16">
         <v>0.61111111111111105</v>
       </c>
@@ -2571,7 +2676,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="16">
         <v>0.61805555555555503</v>
       </c>
@@ -2591,7 +2696,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="16">
         <v>0.75</v>
       </c>
@@ -2611,7 +2716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="16">
         <v>0.75694444444444453</v>
       </c>
@@ -2631,7 +2736,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="16">
         <v>0.76388888888888895</v>
       </c>
@@ -2651,7 +2756,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="16">
         <v>0.77083333333333404</v>
       </c>
@@ -2671,7 +2776,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="16">
         <v>0.77777777777777801</v>
       </c>
@@ -2691,7 +2796,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="16">
         <v>0.78472222222222299</v>
       </c>
@@ -2711,7 +2816,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="16">
         <v>0.79166666666666696</v>
       </c>
@@ -2731,7 +2836,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="16">
         <v>0.79861111111111205</v>
       </c>
@@ -2751,7 +2856,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="16">
         <v>0.80555555555555602</v>
       </c>
@@ -2771,7 +2876,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="16">
         <v>0.812500000000001</v>
       </c>
@@ -2791,7 +2896,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="16">
         <v>0.81944444444444497</v>
       </c>
@@ -2811,7 +2916,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A53" s="16">
         <v>0.82638888888888995</v>
       </c>
@@ -2846,7 +2951,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.9296875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>